<commit_message>
电波暴击(QQ 1106551898)提供音乐 SPACE FIGHT
</commit_message>
<xml_diff>
--- a/Iocp20Coroutine/表/单位.xlsx
+++ b/Iocp20Coroutine/表/单位.xlsx
@@ -1080,7 +1080,7 @@
     <t>圆坑.bin</t>
   </si>
   <si>
-    <t>https://www.rtsgame.online/music/Sc2_T3.mp3</t>
+    <t>https://www.rtsgame.online/music/SPACE FIGHT 低音质.mp3</t>
   </si>
   <si>
     <r>
@@ -4447,7 +4447,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
@@ -4766,7 +4766,7 @@
     <hyperlink ref="E14" r:id="rId4" display="https://www.rtsgame.online/music/Sc2_T2.mp3" tooltip="https://www.rtsgame.online/music/Sc2_T2.mp3"/>
     <hyperlink ref="G14" r:id="rId5" display="https://www.rtsgame.online/图片/地图/ditu4_1_高清.png" tooltip="https://www.rtsgame.online/图片/地图/ditu4_1_高清.png"/>
     <hyperlink ref="G12" r:id="rId6" display="https://www.rtsgame.online/图片/地图/ditu4_8_高清.png"/>
-    <hyperlink ref="E16" r:id="rId7" display="https://www.rtsgame.online/music/Sc2_T3.mp3" tooltip="https://www.rtsgame.online/music/Sc2_T3.mp3"/>
+    <hyperlink ref="E16" r:id="rId7" display="https://www.rtsgame.online/music/SPACE FIGHT 低音质.mp3" tooltip="https://www.rtsgame.online/music/SPACE FIGHT 低音质.mp3"/>
     <hyperlink ref="G16" r:id="rId8" display="https://www.rtsgame.online/图片/地图/ditu_boss2_高清.png" tooltip="https://www.rtsgame.online/图片/地图/ditu_boss2_高清.png"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>